<commit_message>
Fixed distance to limit switch.
</commit_message>
<xml_diff>
--- a/parts/spider_dropper_parts.xlsx
+++ b/parts/spider_dropper_parts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\PrintableParts\spider_dropper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\spider_dropper\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94163865-435F-40BA-83FB-B7EFEA681F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2D331C-D50D-4667-9AD3-BF45B6669610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="789" yWindow="1269" windowWidth="19851" windowHeight="15711" xr2:uid="{92CA6418-27FC-4AD5-98BD-397EC845101D}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{92CA6418-27FC-4AD5-98BD-397EC845101D}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
   <si>
     <t>Spider Dropper Parts</t>
   </si>
@@ -79,9 +79,6 @@
     <t>M3x6mm machine screws</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B0CTQB97J2/</t>
-  </si>
-  <si>
     <t>DC Option</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>Mechanical Parts</t>
   </si>
   <si>
-    <t>Slightly Smarter Electronics</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -311,6 +305,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/adam-tech/RS1-03-G/9832055</t>
+  </si>
+  <si>
+    <t>Slightly Smarter Upgrade</t>
+  </si>
+  <si>
+    <t>M3 hex nuts</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0CTQ36QMW/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0CMGK8MV9/</t>
   </si>
 </sst>
 </file>
@@ -702,15 +708,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49C792C-E920-409F-B110-1A72354C03E4}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="28.3828125" customWidth="1"/>
+    <col min="4" max="4" width="7.61328125" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" customWidth="1"/>
+    <col min="9" max="9" width="8.07421875" customWidth="1"/>
     <col min="11" max="11" width="2.921875" customWidth="1"/>
     <col min="12" max="12" width="10.69140625" customWidth="1"/>
     <col min="13" max="13" width="10.3828125" customWidth="1"/>
@@ -723,13 +732,13 @@
         <v>0</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
@@ -737,19 +746,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>2</v>
@@ -763,12 +772,12 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
         <v>11.99</v>
@@ -777,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1">
         <f>B4*0.1075</f>
@@ -805,7 +814,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <v>11.99</v>
@@ -814,7 +823,7 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E8" si="0">B5*0.1075</f>
@@ -842,7 +851,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>7.19</v>
@@ -851,7 +860,7 @@
         <v>330</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
@@ -882,7 +891,7 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
@@ -907,7 +916,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
         <f>2*35.99</f>
@@ -917,7 +926,7 @@
         <v>2000</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
@@ -940,12 +949,12 @@
         <v>2.7901247499999999</v>
       </c>
       <c r="O8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -975,7 +984,7 @@
     <row r="10" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1"/>
       <c r="E11" s="1"/>
@@ -986,7 +995,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
         <v>18.95</v>
@@ -995,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" ref="E12:E13" si="4">B12*0.1075</f>
@@ -1034,7 +1043,7 @@
         <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="4"/>
@@ -1062,7 +1071,7 @@
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1096,7 +1105,7 @@
     </row>
     <row r="16" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.4">
@@ -1110,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" ref="E17:E19" si="6">B17*0.1075</f>
@@ -1147,7 +1156,7 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="6"/>
@@ -1184,7 +1193,7 @@
         <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="6"/>
@@ -1200,19 +1209,19 @@
         <v>0.1326785</v>
       </c>
       <c r="I19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J19" s="1">
         <f>H19*I19</f>
-        <v>1.061428</v>
-      </c>
-      <c r="O19" t="s">
-        <v>17</v>
+        <v>0.66339250000000005</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1224,15 +1233,15 @@
       <c r="I20" s="3"/>
       <c r="J20" s="4">
         <f>SUM(J17:J19)</f>
-        <v>15.391370500000001</v>
+        <v>14.993335000000002</v>
       </c>
       <c r="M20" s="1">
         <f>J20</f>
-        <v>15.391370500000001</v>
+        <v>14.993335000000002</v>
       </c>
       <c r="N20" s="1">
         <f>J20</f>
-        <v>15.391370500000001</v>
+        <v>14.993335000000002</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1249,12 +1258,12 @@
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1">
         <v>5</v>
@@ -1263,7 +1272,7 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
@@ -1285,12 +1294,12 @@
         <v>2.4980000000000002</v>
       </c>
       <c r="O23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24" s="1">
         <v>15.99</v>
@@ -1299,7 +1308,7 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" ref="E24" si="12">B24*0.1075</f>
@@ -1322,12 +1331,12 @@
         <v>1.7708925</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1">
         <v>2.14</v>
@@ -1336,7 +1345,7 @@
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" ref="E25:E26" si="15">B25*0.1075</f>
@@ -1359,12 +1368,12 @@
         <v>0.23700499999999999</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1">
         <v>6.2</v>
@@ -1373,7 +1382,7 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="15"/>
@@ -1396,12 +1405,12 @@
         <v>0.68664999999999998</v>
       </c>
       <c r="O26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B27" s="1">
         <v>4.01</v>
@@ -1410,7 +1419,7 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" ref="E27" si="16">B27*0.1075</f>
@@ -1433,12 +1442,12 @@
         <v>0.44410749999999999</v>
       </c>
       <c r="O27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B28" s="1">
         <v>2.1</v>
@@ -1447,7 +1456,7 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" ref="E28" si="19">B28*0.1075</f>
@@ -1470,12 +1479,12 @@
         <v>0.23257500000000003</v>
       </c>
       <c r="O28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1">
         <v>2.83</v>
@@ -1484,7 +1493,7 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" ref="E29" si="22">B29*0.1075</f>
@@ -1507,12 +1516,12 @@
         <v>0.31342250000000005</v>
       </c>
       <c r="O29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B30" s="1">
         <v>27.04</v>
@@ -1521,7 +1530,7 @@
         <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" ref="E30" si="25">B30*0.1075</f>
@@ -1544,12 +1553,12 @@
         <v>0.59893600000000002</v>
       </c>
       <c r="O30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B31" s="1">
         <v>1.33</v>
@@ -1558,7 +1567,7 @@
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" ref="E31:E32" si="28">B31*0.1075</f>
@@ -1581,12 +1590,12 @@
         <v>5.8919000000000006E-2</v>
       </c>
       <c r="O31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B32" s="1">
         <v>0.55000000000000004</v>
@@ -1595,7 +1604,7 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="28"/>
@@ -1618,12 +1627,12 @@
         <v>6.0912500000000001E-2</v>
       </c>
       <c r="O32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B33" s="1">
         <v>4.99</v>
@@ -1632,19 +1641,19 @@
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" ref="E33" si="31">B33*0.1075</f>
+        <f t="shared" ref="E33:E35" si="31">B33*0.1075</f>
         <v>0.53642500000000004</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1">
-        <f t="shared" ref="G33" si="32">B33+E33+F33</f>
+        <f t="shared" ref="G33:G35" si="32">B33+E33+F33</f>
         <v>5.5264250000000006</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" ref="H33" si="33">IF(C33&gt;0, G33/C33, 0)</f>
+        <f t="shared" ref="H33:H35" si="33">IF(C33&gt;0, G33/C33, 0)</f>
         <v>0.27632125000000002</v>
       </c>
       <c r="I33">
@@ -1655,66 +1664,106 @@
         <v>0.27632125000000002</v>
       </c>
       <c r="O33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="4">
-        <f>SUM(J23:J33)</f>
-        <v>7.1777412499999995</v>
-      </c>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1">
-        <f>J34</f>
-        <v>7.1777412499999995</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="1"/>
-      <c r="E35" s="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="C34">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="31"/>
+        <v>0.64392499999999997</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1">
+        <f t="shared" si="32"/>
+        <v>6.6339250000000005</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="33"/>
+        <v>0.1326785</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34" s="1">
+        <f>H34*I34</f>
+        <v>0.26535700000000001</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="1">
+        <v>5.49</v>
+      </c>
+      <c r="C35">
+        <v>200</v>
+      </c>
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="31"/>
+        <v>0.59017500000000001</v>
+      </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="G35" s="1">
+        <f t="shared" si="32"/>
+        <v>6.0801750000000006</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="33"/>
+        <v>3.0400875000000004E-2</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="J35" s="1">
+        <f>H35*I35</f>
+        <v>6.0801750000000009E-2</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="36" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="4">
-        <f>SUM(L3:L35)</f>
-        <v>38.006407045454544</v>
-      </c>
-      <c r="M36" s="4">
-        <f>SUM(M3:M35)</f>
-        <v>22.507138545454545</v>
-      </c>
-      <c r="N36" s="4">
-        <f>SUM(N3:N35)</f>
-        <v>29.684879795454545</v>
+      <c r="J36" s="4">
+        <f>SUM(J23:J35)</f>
+        <v>7.5038999999999998</v>
+      </c>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1">
+        <f>J36</f>
+        <v>7.5038999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.4">
@@ -1725,47 +1774,84 @@
       <c r="H37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="J38" s="1"/>
+    <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="4">
+        <f>SUM(L3:L37)</f>
+        <v>38.006407045454544</v>
+      </c>
+      <c r="M38" s="4">
+        <f>SUM(M3:M37)</f>
+        <v>22.109103045454546</v>
+      </c>
+      <c r="N38" s="4">
+        <f>SUM(N3:N37)</f>
+        <v>29.613003045454548</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>23</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="J40" s="1"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A42" s="5"/>
+      <c r="A42" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>92</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A44" s="5"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O24" r:id="rId1" xr:uid="{394BA01E-496A-4B9E-AF12-01E77921BE0E}"/>
     <hyperlink ref="O25" r:id="rId2" xr:uid="{229E0547-4398-43AE-9042-0D4FDFFB3BD5}"/>
+    <hyperlink ref="O19" r:id="rId3" xr:uid="{59869D84-F75A-42B0-B422-BA8AA8AB692E}"/>
+    <hyperlink ref="O35" r:id="rId4" xr:uid="{ED21D2F4-CBE0-426A-A036-B9B33370EF91}"/>
+    <hyperlink ref="O34" r:id="rId5" xr:uid="{916C30C5-416A-439A-9D92-626717DEB750}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1788,40 +1874,40 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>56</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1">
         <v>1.95</v>
@@ -1832,23 +1918,23 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
         <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>64</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -1856,10 +1942,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1">
         <v>1.75</v>
@@ -1867,30 +1953,30 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1">
         <v>1.33</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1">
         <v>0.25</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1">
         <v>2.31</v>
@@ -1901,32 +1987,32 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the parts spreadsheet.
</commit_message>
<xml_diff>
--- a/parts/spider_dropper_parts.xlsx
+++ b/parts/spider_dropper_parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\spider_dropper\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2D331C-D50D-4667-9AD3-BF45B6669610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860F9A35-875B-471C-92C8-6FFC5F09EB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{92CA6418-27FC-4AD5-98BD-397EC845101D}"/>
+    <workbookView xWindow="10971" yWindow="583" windowWidth="19852" windowHeight="15711" xr2:uid="{92CA6418-27FC-4AD5-98BD-397EC845101D}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
-  <si>
-    <t>Spider Dropper Parts</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
   <si>
     <t>Price</t>
   </si>
@@ -55,9 +52,6 @@
     <t>https://www.amazon.com/gp/product/B07TWZ7X38/</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B09L8B1YZC/</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/gp/product/B072BXB2Y8/</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>Tax</t>
   </si>
   <si>
-    <t>elastic string</t>
-  </si>
-  <si>
     <t>MonsterGuts shipping estimated based on commercial USPS Priority Mail Flat Rate.</t>
   </si>
   <si>
@@ -317,6 +308,27 @@
   </si>
   <si>
     <t>https://www.amazon.com/dp/B0CMGK8MV9/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0CZQMZDM8/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B08KZPHDPY/</t>
+  </si>
+  <si>
+    <t>fishing wire for hanging</t>
+  </si>
+  <si>
+    <t>In bulk, cable ties are essentially free.</t>
+  </si>
+  <si>
+    <t>The DC version (including the Slightly Smarter upgrade) requires a 12VDC power supply.</t>
+  </si>
+  <si>
+    <t>Stupidly Simple Spider Dropper Parts</t>
+  </si>
+  <si>
+    <t>The power connector and screw terminal could be omitted in favor of directly wiring pigtail power connectors to the PCB.</t>
   </si>
 </sst>
 </file>
@@ -708,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49C792C-E920-409F-B110-1A72354C03E4}">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -729,55 +741,55 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>11.99</v>
@@ -786,7 +798,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1">
         <f>B4*0.1075</f>
@@ -809,12 +821,12 @@
         <v>3.3197312500000002</v>
       </c>
       <c r="O4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
         <v>11.99</v>
@@ -823,7 +835,7 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E8" si="0">B5*0.1075</f>
@@ -846,52 +858,52 @@
         <v>0.88526166666666672</v>
       </c>
       <c r="O5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="B6" s="1">
-        <v>7.19</v>
+        <v>6.29</v>
       </c>
       <c r="C6">
-        <v>330</v>
+        <v>656</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>0.77292500000000008</v>
+        <v>0.67617499999999997</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>7.9629250000000003</v>
+        <v>6.9661749999999998</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="2"/>
-        <v>2.413007575757576E-2</v>
+        <v>1.0619169207317073E-2</v>
       </c>
       <c r="I6">
         <v>5</v>
       </c>
       <c r="J6" s="1">
         <f>H6*I6</f>
-        <v>0.12065037878787879</v>
+        <v>5.3095846036585362E-2</v>
       </c>
       <c r="O6" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
@@ -916,7 +928,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1">
         <f>2*35.99</f>
@@ -926,7 +938,7 @@
         <v>2000</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
@@ -949,12 +961,12 @@
         <v>2.7901247499999999</v>
       </c>
       <c r="O8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -966,25 +978,25 @@
       <c r="I9" s="3"/>
       <c r="J9" s="4">
         <f>SUM(J4:J8)</f>
-        <v>7.115768045454546</v>
+        <v>7.0482135127032528</v>
       </c>
       <c r="L9" s="1">
         <f>J9</f>
-        <v>7.115768045454546</v>
+        <v>7.0482135127032528</v>
       </c>
       <c r="M9" s="1">
         <f>J9</f>
-        <v>7.115768045454546</v>
+        <v>7.0482135127032528</v>
       </c>
       <c r="N9" s="1">
         <f>J9</f>
-        <v>7.115768045454546</v>
+        <v>7.0482135127032528</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1"/>
       <c r="E11" s="1"/>
@@ -995,7 +1007,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>18.95</v>
@@ -1004,7 +1016,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" ref="E12:E13" si="4">B12*0.1075</f>
@@ -1029,12 +1041,12 @@
         <v>30.537125</v>
       </c>
       <c r="O12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>7.98</v>
@@ -1043,7 +1055,7 @@
         <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="4"/>
@@ -1066,12 +1078,12 @@
         <v>0.35351399999999999</v>
       </c>
       <c r="O13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1105,49 +1117,52 @@
     </row>
     <row r="16" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1">
-        <v>11.99</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" ref="E17:E19" si="6">B17*0.1075</f>
-        <v>1.2889250000000001</v>
+        <v>2.0414249999999998</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1">
         <f t="shared" ref="G17:G19" si="7">B17+E17+F17</f>
-        <v>13.278925000000001</v>
+        <v>21.031424999999999</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" ref="H17:H19" si="8">IF(C17&gt;0, G17/C17, 0)</f>
-        <v>13.278925000000001</v>
+        <v>10.515712499999999</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" s="1">
         <f>H17*I17</f>
-        <v>13.278925000000001</v>
-      </c>
-      <c r="O17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+        <v>10.515712499999999</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="P17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1">
         <v>9.49</v>
@@ -1156,7 +1171,7 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="6"/>
@@ -1179,12 +1194,12 @@
         <v>1.0510174999999999</v>
       </c>
       <c r="O18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1">
         <v>5.99</v>
@@ -1193,7 +1208,7 @@
         <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="6"/>
@@ -1216,12 +1231,12 @@
         <v>0.66339250000000005</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1233,18 +1248,18 @@
       <c r="I20" s="3"/>
       <c r="J20" s="4">
         <f>SUM(J17:J19)</f>
-        <v>14.993335000000002</v>
+        <v>12.2301225</v>
       </c>
       <c r="M20" s="1">
         <f>J20</f>
-        <v>14.993335000000002</v>
+        <v>12.2301225</v>
       </c>
       <c r="N20" s="1">
         <f>J20</f>
-        <v>14.993335000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+        <v>12.2301225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1256,23 +1271,23 @@
       <c r="I21" s="3"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1">
         <v>5</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
@@ -1284,22 +1299,22 @@
       </c>
       <c r="H23" s="1">
         <f t="shared" ref="H23:H26" si="10">IF(C23&gt;0, G23/C23, 0)</f>
-        <v>2.4980000000000002</v>
+        <v>4.9960000000000004</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" ref="J23:J33" si="11">H23*I23</f>
-        <v>2.4980000000000002</v>
+        <v>4.9960000000000004</v>
       </c>
       <c r="O23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B24" s="1">
         <v>15.99</v>
@@ -1308,7 +1323,7 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" ref="E24" si="12">B24*0.1075</f>
@@ -1331,12 +1346,12 @@
         <v>1.7708925</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B25" s="1">
         <v>2.14</v>
@@ -1345,7 +1360,7 @@
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" ref="E25:E26" si="15">B25*0.1075</f>
@@ -1368,12 +1383,12 @@
         <v>0.23700499999999999</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B26" s="1">
         <v>6.2</v>
@@ -1382,7 +1397,7 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="15"/>
@@ -1405,12 +1420,12 @@
         <v>0.68664999999999998</v>
       </c>
       <c r="O26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B27" s="1">
         <v>4.01</v>
@@ -1419,7 +1434,7 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" ref="E27" si="16">B27*0.1075</f>
@@ -1442,12 +1457,12 @@
         <v>0.44410749999999999</v>
       </c>
       <c r="O27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B28" s="1">
         <v>2.1</v>
@@ -1456,7 +1471,7 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" ref="E28" si="19">B28*0.1075</f>
@@ -1479,12 +1494,12 @@
         <v>0.23257500000000003</v>
       </c>
       <c r="O28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1">
         <v>2.83</v>
@@ -1493,7 +1508,7 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" ref="E29" si="22">B29*0.1075</f>
@@ -1516,12 +1531,12 @@
         <v>0.31342250000000005</v>
       </c>
       <c r="O29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1">
         <v>27.04</v>
@@ -1530,7 +1545,7 @@
         <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" ref="E30" si="25">B30*0.1075</f>
@@ -1553,12 +1568,12 @@
         <v>0.59893600000000002</v>
       </c>
       <c r="O30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B31" s="1">
         <v>1.33</v>
@@ -1567,7 +1582,7 @@
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" ref="E31:E32" si="28">B31*0.1075</f>
@@ -1590,12 +1605,12 @@
         <v>5.8919000000000006E-2</v>
       </c>
       <c r="O31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B32" s="1">
         <v>0.55000000000000004</v>
@@ -1604,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="28"/>
@@ -1627,12 +1642,12 @@
         <v>6.0912500000000001E-2</v>
       </c>
       <c r="O32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1">
         <v>4.99</v>
@@ -1641,7 +1656,7 @@
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" ref="E33:E35" si="31">B33*0.1075</f>
@@ -1664,15 +1679,15 @@
         <v>0.27632125000000002</v>
       </c>
       <c r="O33" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B34" s="1">
         <v>5.99</v>
@@ -1681,7 +1696,7 @@
         <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="31"/>
@@ -1704,12 +1719,12 @@
         <v>0.26535700000000001</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="1">
         <v>5.49</v>
@@ -1718,7 +1733,7 @@
         <v>200</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="31"/>
@@ -1741,12 +1756,12 @@
         <v>6.0801750000000009E-2</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1758,12 +1773,12 @@
       <c r="I36" s="3"/>
       <c r="J36" s="4">
         <f>SUM(J23:J35)</f>
-        <v>7.5038999999999998</v>
+        <v>10.001900000000001</v>
       </c>
       <c r="M36" s="1"/>
       <c r="N36" s="1">
         <f>J36</f>
-        <v>7.5038999999999998</v>
+        <v>10.001900000000001</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.4">
@@ -1776,7 +1791,7 @@
     </row>
     <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B38" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1789,15 +1804,15 @@
       <c r="K38" s="3"/>
       <c r="L38" s="4">
         <f>SUM(L3:L37)</f>
-        <v>38.006407045454544</v>
+        <v>37.938852512703249</v>
       </c>
       <c r="M38" s="4">
         <f>SUM(M3:M37)</f>
-        <v>22.109103045454546</v>
+        <v>19.278336012703253</v>
       </c>
       <c r="N38" s="4">
         <f>SUM(N3:N37)</f>
-        <v>29.613003045454548</v>
+        <v>29.280236012703256</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.4">
@@ -1810,7 +1825,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1"/>
       <c r="E40" s="1"/>
@@ -1821,12 +1836,12 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.4">
@@ -1834,12 +1849,27 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1849,9 +1879,10 @@
     <hyperlink ref="O19" r:id="rId3" xr:uid="{59869D84-F75A-42B0-B422-BA8AA8AB692E}"/>
     <hyperlink ref="O35" r:id="rId4" xr:uid="{ED21D2F4-CBE0-426A-A036-B9B33370EF91}"/>
     <hyperlink ref="O34" r:id="rId5" xr:uid="{916C30C5-416A-439A-9D92-626717DEB750}"/>
+    <hyperlink ref="O17" r:id="rId6" xr:uid="{D1850C95-FE4D-4651-A768-4D4B82A92A51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1874,40 +1905,40 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1">
         <v>1.95</v>
@@ -1918,23 +1949,23 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -1942,10 +1973,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1">
         <v>1.75</v>
@@ -1953,30 +1984,30 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1">
         <v>1.33</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1">
         <v>0.25</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1">
         <v>2.31</v>
@@ -1987,32 +2018,32 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>